<commit_message>
Working on Excel for statistics.
</commit_message>
<xml_diff>
--- a/StudentPerformance.xlsx
+++ b/StudentPerformance.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>Student Performance in College: An Analysis*</t>
   </si>
@@ -114,6 +114,24 @@
   </si>
   <si>
     <t>Predictive Statistics</t>
+  </si>
+  <si>
+    <t>Correlations</t>
+  </si>
+  <si>
+    <t>Histograms</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>GPA Bins</t>
+  </si>
+  <si>
+    <t>GPA</t>
   </si>
 </sst>
 </file>
@@ -123,7 +141,14 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -176,8 +201,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +252,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -247,30 +292,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -339,58 +360,236 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="5" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="5" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="6" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="5" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="5" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="4"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="7" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="7" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="5" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="5" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="6" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="5" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="5" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
+    <cellStyle name="20% - Accent1" xfId="7" builtinId="30"/>
+    <cellStyle name="20% - Accent4" xfId="8" builtinId="42"/>
     <cellStyle name="20% - Accent6" xfId="6" builtinId="50"/>
     <cellStyle name="40% - Accent2" xfId="4" builtinId="35"/>
     <cellStyle name="Accent6" xfId="5" builtinId="49"/>
@@ -407,6 +606,942 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>HS GPA</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Frequency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$Q$10:$Q$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$10:$R$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="-2056681744"/>
+        <c:axId val="-2067601472"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2056681744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2067601472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2067601472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2056681744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>26458</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14816</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>470958</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>112183</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -672,10 +1807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:R23"/>
+  <dimension ref="C2:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9:R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,510 +1823,669 @@
     <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:18" ht="20" x14ac:dyDescent="0.25">
-      <c r="E2" s="1" t="s">
+    <row r="2" spans="3:21" ht="20" x14ac:dyDescent="0.25">
+      <c r="E2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
     </row>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C4" s="3" t="s">
+    <row r="4" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
     </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
+    <row r="5" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="8">
         <v>3.2</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>2000</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>3</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="15">
         <v>3.1</v>
       </c>
     </row>
-    <row r="6" spans="3:18" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="6" spans="3:21" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="8">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>1800</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>4</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="15">
         <v>1.9</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="45"/>
+      <c r="O6" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="46"/>
     </row>
-    <row r="7" spans="3:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
+    <row r="7" spans="3:21" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="8">
         <v>2.1</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>1900</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>3</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="15">
         <v>2.5</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="12"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+    <row r="8" spans="3:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="8">
         <v>3.8</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>2200</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>5</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="15">
         <v>3.8</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="14" t="s">
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="12"/>
+      <c r="M8" s="4"/>
+      <c r="O8" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
+    <row r="9" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="8">
         <v>3.9</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>2200</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="15">
         <v>3.2</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9" s="8">
         <f>AVERAGE(D5:D20)</f>
         <v>3.1312499999999996</v>
       </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="17" t="s">
+      <c r="K9" s="3"/>
+      <c r="L9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="10">
         <f>AVERAGE(E5:E20)</f>
         <v>1768.75</v>
       </c>
+      <c r="O9" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="R9" s="26" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
+    <row r="10" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="8">
         <v>3</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>2100</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>3</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="15">
         <v>3.4</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10" s="8">
         <f>MEDIAN(D5:D20)</f>
         <v>3.1500000000000004</v>
       </c>
-      <c r="K10" s="11"/>
-      <c r="L10" s="17" t="s">
+      <c r="K10" s="3"/>
+      <c r="L10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="12">
+      <c r="M10" s="4">
         <f>MEDIAN(E5:E20)</f>
         <v>1750</v>
       </c>
+      <c r="O10" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="47">
+        <v>2</v>
+      </c>
+      <c r="R10" s="24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
+    <row r="11" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="8">
         <v>2.7</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>1700</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>4</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="15">
         <v>2.8</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="3">
         <f>_xlfn.MODE.SNGL(D5:D20)</f>
         <v>3.9</v>
       </c>
-      <c r="K11" s="11"/>
-      <c r="L11" s="17" t="s">
+      <c r="K11" s="3"/>
+      <c r="L11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="M11" s="12">
+      <c r="M11" s="4">
         <f>_xlfn.MODE.SNGL(E5:E20)</f>
         <v>1400</v>
       </c>
+      <c r="O11" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="Q11" s="47">
+        <v>2.5</v>
+      </c>
+      <c r="R11" s="24">
+        <v>4</v>
+      </c>
     </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
+    <row r="12" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="8">
         <v>4</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>2300</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>5</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="15">
         <v>4</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="11">
         <f>_xlfn.VAR.S(D5:D20)</f>
         <v>0.46895833333333786</v>
       </c>
-      <c r="K12" s="11"/>
-      <c r="L12" s="17" t="s">
+      <c r="K12" s="3"/>
+      <c r="L12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="M12" s="12">
+      <c r="M12" s="4">
         <f>_xlfn.VAR.S(E5:E20)</f>
         <v>112958.33333333333</v>
       </c>
+      <c r="O12" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="47">
+        <v>3</v>
+      </c>
+      <c r="R12" s="24">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
+    <row r="13" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="8">
         <v>3.4</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>1500</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>3</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="15">
         <v>3.1</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="11">
         <f>_xlfn.STDEV.S(D5:D20)</f>
         <v>0.68480532513506187</v>
       </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="17" t="s">
+      <c r="K13" s="3"/>
+      <c r="L13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M13" s="20">
+      <c r="M13" s="12">
         <f>_xlfn.STDEV.S(E5:E20)</f>
         <v>336.09274513641816</v>
       </c>
+      <c r="O13" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="Q13" s="47">
+        <v>3.5</v>
+      </c>
+      <c r="R13" s="24">
+        <v>3</v>
+      </c>
     </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
+    <row r="14" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <v>1300</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <v>5</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="15">
         <v>2.8</v>
       </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="12"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="4"/>
+      <c r="O14" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="47">
+        <v>4</v>
+      </c>
+      <c r="R14" s="24">
+        <v>5</v>
+      </c>
     </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
+    <row r="15" spans="3:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="8">
         <v>2.9</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <v>1400</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <v>3</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="15">
         <v>2</v>
       </c>
-      <c r="I15" s="21" t="s">
+      <c r="I15" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="22" t="s">
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="12"/>
+      <c r="M15" s="4"/>
+      <c r="Q15" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="R15" s="25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
+    <row r="16" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="8">
         <v>3.1</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <v>1400</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>4</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="15">
         <v>3.1</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="11">
         <f>AVERAGE(F5:F20)</f>
         <v>3.4375</v>
       </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="17" t="s">
+      <c r="K16" s="3"/>
+      <c r="L16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="M16" s="23">
+      <c r="M16" s="15">
         <f>AVERAGE(G5:G20)</f>
         <v>3.0625000000000004</v>
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="8">
         <v>3.9</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <v>1600</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>2</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="15">
         <v>3.6</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="I17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="3">
         <f>MEDIAN(F5:F20)</f>
         <v>3</v>
       </c>
-      <c r="K17" s="11"/>
-      <c r="L17" s="17" t="s">
+      <c r="K17" s="3"/>
+      <c r="L17" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M17" s="23">
+      <c r="M17" s="15">
         <f>MEDIAN(G5:G20)</f>
         <v>3.1</v>
       </c>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="8">
         <v>4</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>2000</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>2</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="15">
         <v>3.7</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="I18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="3">
         <f>_xlfn.MODE.SNGL(F5:F20)</f>
         <v>3</v>
       </c>
-      <c r="K18" s="11"/>
-      <c r="L18" s="17" t="s">
+      <c r="K18" s="3"/>
+      <c r="L18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="M18" s="12">
+      <c r="M18" s="4">
         <f>_xlfn.MODE.SNGL(G5:G20)</f>
         <v>3.1</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <v>1400</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>5</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="15">
         <v>2.8</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="I19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="11">
         <f>_xlfn.VAR.S(F5:F20)</f>
         <v>1.4624999999999999</v>
       </c>
-      <c r="K19" s="11"/>
-      <c r="L19" s="17" t="s">
+      <c r="K19" s="3"/>
+      <c r="L19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="M19" s="12">
+      <c r="M19" s="4">
         <f>_xlfn.VAR.S(G5:G20)</f>
         <v>0.35183333333332978</v>
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
+      <c r="C20" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="41">
         <v>3.4</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="18">
         <v>1500</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="18">
         <v>3</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="42">
         <v>3.2</v>
       </c>
-      <c r="I20" s="24" t="s">
+      <c r="I20" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20" s="17">
         <f>_xlfn.STDEV.S(F5:F20)</f>
         <v>1.2093386622447824</v>
       </c>
-      <c r="K20" s="26"/>
-      <c r="L20" s="27" t="s">
+      <c r="K20" s="18"/>
+      <c r="L20" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="28">
+      <c r="M20" s="20">
         <f>_xlfn.STDEV.S(G5:G20)</f>
         <v>0.59315540403281308</v>
       </c>
     </row>
     <row r="23" spans="3:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="I23" s="5" t="s">
+      <c r="H23" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="J23" s="5"/>
+      <c r="I23" s="23"/>
+    </row>
+    <row r="24" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="36"/>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C26" s="28"/>
+      <c r="D26" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C27" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="24">
+        <v>1</v>
+      </c>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="31"/>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C28" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="24">
+        <v>0.49983757192377043</v>
+      </c>
+      <c r="E28" s="24">
+        <v>1</v>
+      </c>
+      <c r="F28" s="24"/>
+      <c r="G28" s="31"/>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C29" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="24">
+        <v>-0.41205728231566746</v>
+      </c>
+      <c r="E29" s="24">
+        <v>-0.1773486088326881</v>
+      </c>
+      <c r="F29" s="24">
+        <v>1</v>
+      </c>
+      <c r="G29" s="31"/>
+    </row>
+    <row r="30" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="25">
+        <v>0.78430942096257783</v>
+      </c>
+      <c r="E30" s="25">
+        <v>0.50537927193397958</v>
+      </c>
+      <c r="F30" s="25">
+        <v>-4.9954058798400598E-2</v>
+      </c>
+      <c r="G30" s="33">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <sortState ref="Q10:Q14">
+    <sortCondition ref="Q10"/>
+  </sortState>
+  <mergeCells count="6">
     <mergeCell ref="E2:J2"/>
     <mergeCell ref="N4:R4"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="O6:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on Excel data analysis example.
</commit_message>
<xml_diff>
--- a/StudentPerformance.xlsx
+++ b/StudentPerformance.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>Student Performance in College: An Analysis*</t>
   </si>
@@ -132,6 +132,90 @@
   </si>
   <si>
     <t>GPA</t>
+  </si>
+  <si>
+    <t>SAT Bins</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>RESIDUAL OUTPUT</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>Residuals</t>
+  </si>
+  <si>
+    <t>Predicted College GPA</t>
   </si>
 </sst>
 </file>
@@ -210,7 +294,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,8 +348,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -494,6 +584,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -506,7 +644,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -528,15 +666,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="5" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -555,6 +684,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="7" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -564,12 +712,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -582,8 +724,52 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -809,11 +995,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-2056681744"/>
-        <c:axId val="-2067601472"/>
+        <c:axId val="2100620064"/>
+        <c:axId val="2100623104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2056681744"/>
+        <c:axId val="2100620064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +1041,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2067601472"/>
+        <c:crossAx val="2100623104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -863,7 +1049,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2067601472"/>
+        <c:axId val="2100623104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +1099,377 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056681744"/>
+        <c:crossAx val="2100620064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SAT</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Frequency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$Q$34:$Q$39</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>More</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$34:$R$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="-2113162752"/>
+        <c:axId val="-2082652304"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2113162752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2082652304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2082652304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2113162752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1013,7 +1569,543 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1536,6 +2628,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>5291</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>449791</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>154517</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1807,55 +2929,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:U30"/>
+  <dimension ref="C2:U73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9:R14"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:21" ht="20" x14ac:dyDescent="0.25">
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="4" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="N4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
     </row>
     <row r="5" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1890,22 +3013,22 @@
       <c r="G6" s="15">
         <v>1.9</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="45"/>
-      <c r="O6" s="46" t="s">
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="47"/>
+      <c r="O6" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
-      <c r="S6" s="46"/>
-      <c r="T6" s="46"/>
-      <c r="U6" s="46"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="48"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="48"/>
+      <c r="U6" s="48"/>
     </row>
     <row r="7" spans="3:21" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
@@ -1989,13 +3112,13 @@
         <f>AVERAGE(E5:E20)</f>
         <v>1768.75</v>
       </c>
-      <c r="O9" s="48" t="s">
+      <c r="O9" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="Q9" s="26" t="s">
+      <c r="Q9" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="R9" s="26" t="s">
+      <c r="R9" s="49" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2033,10 +3156,10 @@
       <c r="O10" s="1">
         <v>2</v>
       </c>
-      <c r="Q10" s="47">
+      <c r="Q10" s="37">
         <v>2</v>
       </c>
-      <c r="R10" s="24">
+      <c r="R10" s="21">
         <v>0</v>
       </c>
     </row>
@@ -2074,10 +3197,10 @@
       <c r="O11" s="1">
         <v>2.5</v>
       </c>
-      <c r="Q11" s="47">
+      <c r="Q11" s="37">
         <v>2.5</v>
       </c>
-      <c r="R11" s="24">
+      <c r="R11" s="21">
         <v>4</v>
       </c>
     </row>
@@ -2115,10 +3238,10 @@
       <c r="O12" s="1">
         <v>3</v>
       </c>
-      <c r="Q12" s="47">
+      <c r="Q12" s="37">
         <v>3</v>
       </c>
-      <c r="R12" s="24">
+      <c r="R12" s="21">
         <v>3</v>
       </c>
     </row>
@@ -2156,10 +3279,10 @@
       <c r="O13" s="1">
         <v>3.5</v>
       </c>
-      <c r="Q13" s="47">
+      <c r="Q13" s="37">
         <v>3.5</v>
       </c>
-      <c r="R13" s="24">
+      <c r="R13" s="21">
         <v>3</v>
       </c>
     </row>
@@ -2187,10 +3310,10 @@
       <c r="O14" s="1">
         <v>4</v>
       </c>
-      <c r="Q14" s="47">
+      <c r="Q14" s="37">
         <v>4</v>
       </c>
-      <c r="R14" s="24">
+      <c r="R14" s="21">
         <v>5</v>
       </c>
     </row>
@@ -2219,10 +3342,10 @@
         <v>22</v>
       </c>
       <c r="M15" s="4"/>
-      <c r="Q15" s="25" t="s">
+      <c r="Q15" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="R15" s="25">
+      <c r="R15" s="22">
         <v>0</v>
       </c>
     </row>
@@ -2258,7 +3381,7 @@
         <v>3.0625000000000004</v>
       </c>
     </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
@@ -2290,7 +3413,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
@@ -2322,7 +3445,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2354,11 +3477,11 @@
         <v>0.35183333333332978</v>
       </c>
     </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C20" s="40" t="s">
+    <row r="20" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C20" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="35">
         <v>3.4</v>
       </c>
       <c r="E20" s="18">
@@ -2367,7 +3490,7 @@
       <c r="F20" s="18">
         <v>3</v>
       </c>
-      <c r="G20" s="42">
+      <c r="G20" s="36">
         <v>3.2</v>
       </c>
       <c r="I20" s="16" t="s">
@@ -2386,98 +3509,853 @@
         <v>0.59315540403281308</v>
       </c>
     </row>
-    <row r="23" spans="3:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="H23" s="23" t="s">
+    <row r="23" spans="3:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="H23" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="I23" s="23"/>
-    </row>
-    <row r="24" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="34" t="s">
+      <c r="I23" s="41"/>
+    </row>
+    <row r="24" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="36"/>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C26" s="28"/>
-      <c r="D26" s="27" t="s">
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="44"/>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C26" s="25"/>
+      <c r="D26" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="27" t="s">
+      <c r="F26" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C27" s="30" t="s">
+    <row r="27" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C27" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="21">
         <v>1</v>
       </c>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="31"/>
-    </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C28" s="30" t="s">
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="28"/>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C28" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="21">
         <v>0.49983757192377043</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28" s="21">
         <v>1</v>
       </c>
-      <c r="F28" s="24"/>
-      <c r="G28" s="31"/>
-    </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C29" s="30" t="s">
+      <c r="F28" s="21"/>
+      <c r="G28" s="28"/>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C29" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="21">
         <v>-0.41205728231566746</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="21">
         <v>-0.1773486088326881</v>
       </c>
-      <c r="F29" s="24">
+      <c r="F29" s="21">
         <v>1</v>
       </c>
-      <c r="G29" s="31"/>
-    </row>
-    <row r="30" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="32" t="s">
+      <c r="G29" s="28"/>
+    </row>
+    <row r="30" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="25">
+      <c r="D30" s="22">
         <v>0.78430942096257783</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="22">
         <v>0.50537927193397958</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="22">
         <v>-4.9954058798400598E-2</v>
       </c>
-      <c r="G30" s="33">
+      <c r="G30" s="30">
         <v>1</v>
       </c>
     </row>
+    <row r="32" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O32" s="50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C33" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="55"/>
+      <c r="K33" s="56"/>
+      <c r="O33" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q33" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="R33" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="2"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="4"/>
+      <c r="O34">
+        <v>1500</v>
+      </c>
+      <c r="Q34" s="51">
+        <v>1500</v>
+      </c>
+      <c r="R34" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C35" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="53"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="4"/>
+      <c r="O35">
+        <v>1700</v>
+      </c>
+      <c r="Q35" s="51">
+        <v>1700</v>
+      </c>
+      <c r="R35" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C36" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="21">
+        <v>0.79515351561186909</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="4"/>
+      <c r="O36">
+        <v>1900</v>
+      </c>
+      <c r="Q36" s="51">
+        <v>1900</v>
+      </c>
+      <c r="R36" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C37" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="21">
+        <v>0.63226911338991487</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="4"/>
+      <c r="O37">
+        <v>2100</v>
+      </c>
+      <c r="Q37" s="51">
+        <v>2100</v>
+      </c>
+      <c r="R37" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C38" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="21">
+        <v>0.57569513083451718</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="4"/>
+      <c r="O38">
+        <v>2300</v>
+      </c>
+      <c r="Q38" s="51">
+        <v>2300</v>
+      </c>
+      <c r="R38" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="21">
+        <v>0.38637364877545116</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="4"/>
+      <c r="Q39" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="R39" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="22">
+        <v>16</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C41" s="2"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="68"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="68"/>
+      <c r="H42" s="68"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="4"/>
+    </row>
+    <row r="43" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C43" s="60"/>
+      <c r="D43" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C44" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="21">
+        <v>2</v>
+      </c>
+      <c r="E44" s="21">
+        <v>3.3368002459152759</v>
+      </c>
+      <c r="F44" s="21">
+        <v>1.668400122957638</v>
+      </c>
+      <c r="G44" s="21">
+        <v>11.175969674236596</v>
+      </c>
+      <c r="H44" s="21">
+        <v>1.4994973670312281E-3</v>
+      </c>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="4"/>
+    </row>
+    <row r="45" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C45" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="21">
+        <v>13</v>
+      </c>
+      <c r="E45" s="21">
+        <v>1.9406997540847239</v>
+      </c>
+      <c r="F45" s="21">
+        <v>0.1492845964680557</v>
+      </c>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="4"/>
+    </row>
+    <row r="46" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="22">
+        <v>15</v>
+      </c>
+      <c r="E46" s="22">
+        <v>5.2774999999999999</v>
+      </c>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="2"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="4"/>
+    </row>
+    <row r="48" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C48" s="60"/>
+      <c r="D48" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G48" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H48" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I48" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="J48" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="K48" s="61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C49" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="21">
+        <v>0.66846978904970977</v>
+      </c>
+      <c r="E49" s="21">
+        <v>0.57879270396198246</v>
+      </c>
+      <c r="F49" s="21">
+        <v>1.1549381747106779</v>
+      </c>
+      <c r="G49" s="21">
+        <v>0.26890406165034919</v>
+      </c>
+      <c r="H49" s="21">
+        <v>-0.58193582717910508</v>
+      </c>
+      <c r="I49" s="21">
+        <v>1.9188754052785246</v>
+      </c>
+      <c r="J49" s="21">
+        <v>-0.58193582717910508</v>
+      </c>
+      <c r="K49" s="62">
+        <v>1.9188754052785246</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C50" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="21">
+        <v>0.61392350203484791</v>
+      </c>
+      <c r="E50" s="21">
+        <v>0.1681965541752459</v>
+      </c>
+      <c r="F50" s="21">
+        <v>3.6500361439937352</v>
+      </c>
+      <c r="G50" s="21">
+        <v>2.9371269542425443E-3</v>
+      </c>
+      <c r="H50" s="21">
+        <v>0.25055693826960063</v>
+      </c>
+      <c r="I50" s="21">
+        <v>0.97729006580009514</v>
+      </c>
+      <c r="J50" s="21">
+        <v>0.25055693826960063</v>
+      </c>
+      <c r="K50" s="62">
+        <v>0.97729006580009514</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="22">
+        <v>2.6667547432009797E-4</v>
+      </c>
+      <c r="E51" s="22">
+        <v>3.4270866490088646E-4</v>
+      </c>
+      <c r="F51" s="22">
+        <v>0.77814044881888889</v>
+      </c>
+      <c r="G51" s="22">
+        <v>0.45041725502162633</v>
+      </c>
+      <c r="H51" s="22">
+        <v>-4.7370158362998758E-4</v>
+      </c>
+      <c r="I51" s="22">
+        <v>1.0070525322701835E-3</v>
+      </c>
+      <c r="J51" s="22">
+        <v>-4.7370158362998758E-4</v>
+      </c>
+      <c r="K51" s="63">
+        <v>1.0070525322701835E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C52" s="2"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="4"/>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C53" s="2"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="4"/>
+    </row>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C54" s="2"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="4"/>
+    </row>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C55" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="D55" s="70"/>
+      <c r="E55" s="70"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="4"/>
+    </row>
+    <row r="56" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="2"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="4"/>
+    </row>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C57" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="4"/>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C58" s="58">
+        <v>1</v>
+      </c>
+      <c r="D58" s="21">
+        <v>3.1663759442014197</v>
+      </c>
+      <c r="E58" s="21">
+        <v>-6.6375944201419568E-2</v>
+      </c>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="4"/>
+    </row>
+    <row r="59" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C59" s="58">
+        <v>2</v>
+      </c>
+      <c r="D59" s="21">
+        <v>2.5605096975060362</v>
+      </c>
+      <c r="E59" s="21">
+        <v>-0.66050969750603628</v>
+      </c>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="4"/>
+    </row>
+    <row r="60" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C60" s="58">
+        <v>3</v>
+      </c>
+      <c r="D60" s="21">
+        <v>2.4643925445310764</v>
+      </c>
+      <c r="E60" s="21">
+        <v>3.5607455468923632E-2</v>
+      </c>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="4"/>
+    </row>
+    <row r="61" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C61" s="58">
+        <v>4</v>
+      </c>
+      <c r="D61" s="21">
+        <v>3.5880651402863473</v>
+      </c>
+      <c r="E61" s="21">
+        <v>0.21193485971365256</v>
+      </c>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="4"/>
+    </row>
+    <row r="62" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C62" s="58">
+        <v>5</v>
+      </c>
+      <c r="D62" s="21">
+        <v>3.6494574904898318</v>
+      </c>
+      <c r="E62" s="21">
+        <v>-0.44945749048983163</v>
+      </c>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="4"/>
+    </row>
+    <row r="63" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C63" s="58">
+        <v>6</v>
+      </c>
+      <c r="D63" s="21">
+        <v>3.0702587912264594</v>
+      </c>
+      <c r="E63" s="21">
+        <v>0.32974120877354052</v>
+      </c>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="4"/>
+    </row>
+    <row r="64" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C64" s="58">
+        <v>7</v>
+      </c>
+      <c r="D64" s="21">
+        <v>2.7794115508879655</v>
+      </c>
+      <c r="E64" s="21">
+        <v>2.0588449112034279E-2</v>
+      </c>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="4"/>
+    </row>
+    <row r="65" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C65" s="58">
+        <v>8</v>
+      </c>
+      <c r="D65" s="21">
+        <v>3.737517388125327</v>
+      </c>
+      <c r="E65" s="21">
+        <v>0.26248261187467303</v>
+      </c>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="4"/>
+    </row>
+    <row r="66" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C66" s="58">
+        <v>9</v>
+      </c>
+      <c r="D66" s="21">
+        <v>3.1558229074483397</v>
+      </c>
+      <c r="E66" s="21">
+        <v>-5.582290744833962E-2</v>
+      </c>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="4"/>
+    </row>
+    <row r="67" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C67" s="58">
+        <v>10</v>
+      </c>
+      <c r="D67" s="21">
+        <v>2.3657796101425026</v>
+      </c>
+      <c r="E67" s="21">
+        <v>0.43422038985749722</v>
+      </c>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="4"/>
+    </row>
+    <row r="68" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C68" s="58">
+        <v>11</v>
+      </c>
+      <c r="D68" s="21">
+        <v>2.8221936089989059</v>
+      </c>
+      <c r="E68" s="21">
+        <v>-0.82219360899890592</v>
+      </c>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="4"/>
+    </row>
+    <row r="69" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C69" s="58">
+        <v>12</v>
+      </c>
+      <c r="D69" s="21">
+        <v>2.944978309405875</v>
+      </c>
+      <c r="E69" s="21">
+        <v>0.15502169059412507</v>
+      </c>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="4"/>
+    </row>
+    <row r="70" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C70" s="58">
+        <v>13</v>
+      </c>
+      <c r="D70" s="21">
+        <v>3.4894522058977731</v>
+      </c>
+      <c r="E70" s="21">
+        <v>0.11054779410222704</v>
+      </c>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="4"/>
+    </row>
+    <row r="71" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C71" s="58">
+        <v>14</v>
+      </c>
+      <c r="D71" s="21">
+        <v>3.6575147458292978</v>
+      </c>
+      <c r="E71" s="21">
+        <v>4.2485254170702369E-2</v>
+      </c>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="4"/>
+    </row>
+    <row r="72" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C72" s="58">
+        <v>15</v>
+      </c>
+      <c r="D72" s="21">
+        <v>2.3924471575745123</v>
+      </c>
+      <c r="E72" s="21">
+        <v>0.4075528424254875</v>
+      </c>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="4"/>
+    </row>
+    <row r="73" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C73" s="64">
+        <v>16</v>
+      </c>
+      <c r="D73" s="65">
+        <v>3.1558229074483397</v>
+      </c>
+      <c r="E73" s="65">
+        <v>4.4177092551660468E-2</v>
+      </c>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+      <c r="J73" s="18"/>
+      <c r="K73" s="66"/>
+    </row>
   </sheetData>
-  <sortState ref="Q10:Q14">
-    <sortCondition ref="Q10"/>
+  <sortState ref="Q34:Q38">
+    <sortCondition ref="Q34"/>
   </sortState>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="C33:K33"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C42:H42"/>
     <mergeCell ref="E2:J2"/>
     <mergeCell ref="N4:R4"/>
     <mergeCell ref="H23:I23"/>

</xml_diff>